<commit_message>
New domestic and user data
</commit_message>
<xml_diff>
--- a/user-data/gov-revenue-pc-gdp/gov-revenue-pc-gdp.xlsx
+++ b/user-data/gov-revenue-pc-gdp/gov-revenue-pc-gdp.xlsx
@@ -18042,7 +18042,7 @@
         <v>2014</v>
       </c>
       <c r="D1225" t="n">
-        <v>19.0151515151515</v>
+        <v>18.030303030303</v>
       </c>
     </row>
     <row r="1226">
@@ -22358,7 +22358,7 @@
         <v>2014</v>
       </c>
       <c r="D1542" t="n">
-        <v>9.48717948717949</v>
+        <v>9.52991452991453</v>
       </c>
     </row>
     <row r="1543">
@@ -31847,7 +31847,7 @@
         <v>17</v>
       </c>
       <c r="Q83" t="n">
-        <v>19.0151515151515</v>
+        <v>18.030303030303</v>
       </c>
     </row>
     <row r="84">
@@ -32799,7 +32799,7 @@
         <v>10.7042253521127</v>
       </c>
       <c r="Q103" t="n">
-        <v>9.48717948717949</v>
+        <v>9.52991452991453</v>
       </c>
     </row>
     <row r="104">

</xml_diff>